<commit_message>
targets now sorted by priority
</commit_message>
<xml_diff>
--- a/target_observability/EarlyScienceObservability_custom_constraint.xlsx
+++ b/target_observability/EarlyScienceObservability_custom_constraint.xlsx
@@ -569,27 +569,28 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="1" t="inlineStr"/>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>RCW36
+          <t>NGC3199
+W28
+M20
+RCW36
+RCW86
 Pencil
-NGC3199
-RCW86
-G316.75
+G316.75
+M8
+Baades
+NGC6388</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>NGC3199
 W28
 M20
-M8
-Baades
-NGC6388</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>NGC3199
-RCW86
-G316.75
-W28
-M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -597,47 +598,47 @@
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
 OmegaCen
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
+          <t>W28
+M20
 OmegaCen
+RCW86
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -645,10 +646,10 @@
       </c>
       <c r="H2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -658,8 +659,8 @@
         <is>
           <t>W28
 M20
-M8
-NGC6822
+NGC6822
+M8
 Baades
 NGC6388
 AV255</t>
@@ -669,8 +670,8 @@
         <is>
           <t>W28
 M20
-M8
-NGC6822
+NGC6822
+M8
 Baades
 NGC6388
 AV255</t>
@@ -800,76 +801,77 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="1" t="inlineStr"/>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>RCW36
+          <t>NGC3199
+W28
+M20
+OmegaCen
+RCW36
+RCW86
 Pencil
-NGC3199
-RCW86
-G316.75
+G316.75
+M8
+Baades
+NGC6388</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>NGC3199
 W28
 M20
-M8
+RCW86
+G316.75
+M8
+Baades
+NGC6388</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>W28
+M20
+RCW86
+NGC6822
+G316.75
+M8
+Baades
+NGC6388</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>W28
+M20
+RCW86
+NGC6822
+G316.75
+M8
+Baades
+NGC6388</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>W28
+M20
 OmegaCen
-Baades
-NGC6388</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>NGC3199
-RCW86
-G316.75
-W28
-M20
-M8
-Baades
-NGC6388</t>
-        </is>
-      </c>
-      <c r="D2" s="1" t="inlineStr">
-        <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
-Baades
-NGC6388</t>
-        </is>
-      </c>
-      <c r="E2" s="1" t="inlineStr">
-        <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
-Baades
-NGC6388</t>
-        </is>
-      </c>
-      <c r="F2" s="1" t="inlineStr">
-        <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
-OmegaCen
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -877,10 +879,10 @@
       </c>
       <c r="H2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388
@@ -1029,91 +1031,92 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="1" t="inlineStr"/>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>RCW36
+          <t>NGC3199
+W28
+M20
+OmegaCen
+RCW36
+RCW86
 Pencil
-NGC3199
-RCW86
-G316.75
+G316.75
+M8
+Baades
+NGC6388</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>NGC3199
 W28
 M20
-M8
+RCW86
+G316.75
+M8
+Baades
+NGC6388</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>W28
+M20
+RCW86
+NGC6822
+G316.75
+M8
+Baades
+NGC6388</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>W28
+M20
 OmegaCen
-Baades
-NGC6388</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>NGC3199
-RCW86
-G316.75
-W28
-M20
-M8
-Baades
-NGC6388</t>
-        </is>
-      </c>
-      <c r="D2" s="1" t="inlineStr">
-        <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
-Baades
-NGC6388</t>
-        </is>
-      </c>
-      <c r="E2" s="1" t="inlineStr">
-        <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+RCW86
+NGC6822
+G316.75
+M8
+Baades
+NGC6388</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>W28
+M20
 OmegaCen
-Baades
-NGC6388</t>
-        </is>
-      </c>
-      <c r="F2" s="1" t="inlineStr">
-        <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
-OmegaCen
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="H2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
@@ -1122,8 +1125,8 @@
         <is>
           <t>W28
 M20
-M8
-NGC6822
+NGC6822
+M8
 Baades
 NGC6388</t>
         </is>
@@ -1137,6 +1140,7 @@
 NGC6388</t>
         </is>
       </c>
+      <c r="K2" s="1" t="inlineStr"/>
       <c r="L2" s="1" t="inlineStr">
         <is>
           <t>N44</t>
@@ -1251,15 +1255,16 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="1" t="inlineStr"/>
       <c r="B2" s="1" t="inlineStr">
         <is>
           <t>NGC3199
-RCW86
-G316.75
 W28
 M20
-M8
 OmegaCen
+RCW86
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
@@ -1267,10 +1272,10 @@
       <c r="C2" s="1" t="inlineStr">
         <is>
           <t>NGC3199
-RCW86
-G316.75
 W28
 M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -1278,61 +1283,61 @@
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
 OmegaCen
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
 OmegaCen
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
 OmegaCen
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="H2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -1352,8 +1357,8 @@
         <is>
           <t>W28
 M20
-M8
-NGC6822
+NGC6822
+M8
 Baades
 NGC6388
 AV255</t>
@@ -1480,13 +1485,14 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="1" t="inlineStr"/>
       <c r="B2" s="1" t="inlineStr">
         <is>
           <t>NGC3199
-RCW86
-G316.75
 W28
 M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -1495,60 +1501,60 @@
       <c r="C2" s="1" t="inlineStr">
         <is>
           <t>NGC3199
-RCW86
-G316.75
 W28
 M20
-M8
 OmegaCen
+RCW86
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
 OmegaCen
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
 OmegaCen
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
+          <t>W28
+M20
 OmegaCen
+RCW86
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -1567,8 +1573,8 @@
         <is>
           <t>W28
 M20
-M8
-NGC6822
+NGC6822
+M8
 Baades
 NGC6388</t>
         </is>
@@ -1577,12 +1583,13 @@
         <is>
           <t>W28
 M20
-M8
-NGC6822
-Baades
-NGC6388</t>
-        </is>
-      </c>
+NGC6822
+M8
+Baades
+NGC6388</t>
+        </is>
+      </c>
+      <c r="K2" s="1" t="inlineStr"/>
       <c r="L2" s="1" t="inlineStr">
         <is>
           <t>N44
@@ -1698,13 +1705,14 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="1" t="inlineStr"/>
       <c r="B2" s="1" t="inlineStr">
         <is>
           <t>NGC3199
-RCW86
-G316.75
 W28
 M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -1713,60 +1721,60 @@
       <c r="C2" s="1" t="inlineStr">
         <is>
           <t>NGC3199
-RCW86
-G316.75
 W28
 M20
-M8
 OmegaCen
+RCW86
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
+          <t>W28
+M20
 OmegaCen
+RCW86
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
+          <t>W28
+M20
 OmegaCen
+RCW86
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
@@ -1775,8 +1783,8 @@
         <is>
           <t>W28
 M20
-M8
-NGC6822
+NGC6822
+M8
 Baades
 NGC6388
 AV255</t>
@@ -1925,13 +1933,14 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="1" t="inlineStr"/>
       <c r="B2" s="1" t="inlineStr">
         <is>
           <t>NGC3199
-RCW86
-G316.75
 W28
 M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -1940,60 +1949,60 @@
       <c r="C2" s="1" t="inlineStr">
         <is>
           <t>NGC3199
-RCW86
-G316.75
 W28
 M20
-M8
 OmegaCen
+RCW86
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
 OmegaCen
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
 OmegaCen
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
+          <t>W28
+M20
 OmegaCen
+RCW86
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -2003,8 +2012,8 @@
         <is>
           <t>W28
 M20
-M8
-NGC6822
+NGC6822
+M8
 Baades
 NGC6388
 AV255</t>
@@ -2014,8 +2023,8 @@
         <is>
           <t>W28
 M20
-M8
-NGC6822
+NGC6822
+M8
 Baades
 NGC6388
 AV255</t>
@@ -2025,8 +2034,8 @@
         <is>
           <t>W28
 M20
-M8
-NGC6822
+NGC6822
+M8
 Baades
 NGC6388
 AV255</t>
@@ -2156,13 +2165,14 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="1" t="inlineStr"/>
       <c r="B2" s="1" t="inlineStr">
         <is>
           <t>NGC3199
-RCW86
-G316.75
 W28
 M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -2171,10 +2181,10 @@
       <c r="C2" s="1" t="inlineStr">
         <is>
           <t>NGC3199
-RCW86
-G316.75
 W28
 M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -2182,51 +2192,51 @@
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
 OmegaCen
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
 OmegaCen
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
 OmegaCen
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
@@ -2253,8 +2263,8 @@
         <is>
           <t>W28
 M20
-M8
-NGC6822
+NGC6822
+M8
 Baades
 NGC6388</t>
         </is>
@@ -2381,13 +2391,14 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="1" t="inlineStr"/>
       <c r="B2" s="1" t="inlineStr">
         <is>
           <t>NGC3199
-RCW86
-G316.75
 W28
 M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -2396,10 +2407,10 @@
       <c r="C2" s="1" t="inlineStr">
         <is>
           <t>NGC3199
-RCW86
-G316.75
 W28
 M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -2407,10 +2418,10 @@
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -2418,10 +2429,10 @@
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -2429,24 +2440,24 @@
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
@@ -2455,8 +2466,8 @@
         <is>
           <t>W28
 M20
-M8
-NGC6822
+NGC6822
+M8
 Baades
 NGC6388
 AV255</t>
@@ -2507,8 +2518,8 @@
       <c r="N2" s="1" t="inlineStr">
         <is>
           <t>N44
+S308
 30Dor
-S308
 LMCclusters1
 LMCclusters2</t>
         </is>
@@ -2606,13 +2617,14 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="1" t="inlineStr"/>
       <c r="B2" s="1" t="inlineStr">
         <is>
           <t>NGC3199
-RCW86
-G316.75
 W28
 M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -2621,10 +2633,10 @@
       <c r="C2" s="1" t="inlineStr">
         <is>
           <t>NGC3199
-RCW86
-G316.75
 W28
 M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -2632,10 +2644,10 @@
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -2643,10 +2655,10 @@
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -2654,10 +2666,10 @@
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -2665,12 +2677,12 @@
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
@@ -2679,8 +2691,8 @@
         <is>
           <t>W28
 M20
-M8
-NGC6822
+NGC6822
+M8
 Baades
 NGC6388</t>
         </is>
@@ -2689,8 +2701,8 @@
         <is>
           <t>W28
 M20
-M8
-NGC6822
+NGC6822
+M8
 Baades
 NGC6388</t>
         </is>
@@ -2729,8 +2741,8 @@
       <c r="N2" s="1" t="inlineStr">
         <is>
           <t>N44
+S308
 30Dor
-S308
 LMCclusters2
 AV255</t>
         </is>
@@ -2828,83 +2840,84 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="1" t="inlineStr"/>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>RCW36
+          <t>NGC3199
+OmegaCen
+RCW36
+RCW86
 Pencil
-NGC3199
-RCW86
-G316.75
+G316.75
+NGC6388</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>NGC3199
+W28
+M20
+RCW86
+G316.75
+M8
+Baades
+NGC6388</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>NGC3199
+W28
+M20
+RCW86
+G316.75
+M8
+Baades
+NGC6388</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>W28
+M20
+RCW86
+NGC6822
+G316.75
+M8
+Baades
+NGC6388</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>W28
+M20
 OmegaCen
-NGC6388</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>NGC3199
-RCW86
-G316.75
-W28
-M20
-M8
-Baades
-NGC6388</t>
-        </is>
-      </c>
-      <c r="D2" s="1" t="inlineStr">
-        <is>
-          <t>NGC3199
-RCW86
-G316.75
-W28
-M20
-M8
-Baades
-NGC6388</t>
-        </is>
-      </c>
-      <c r="E2" s="1" t="inlineStr">
-        <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
-Baades
-NGC6388</t>
-        </is>
-      </c>
-      <c r="F2" s="1" t="inlineStr">
-        <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
+RCW86
+G316.75
+M8
+Baades
+NGC6388</t>
+        </is>
+      </c>
+      <c r="G2" s="1" t="inlineStr">
+        <is>
+          <t>W28
+M20
 OmegaCen
-Baades
-NGC6388</t>
-        </is>
-      </c>
-      <c r="G2" s="1" t="inlineStr">
-        <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-OmegaCen
+RCW86
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="H2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -2914,8 +2927,8 @@
         <is>
           <t>W28
 M20
-M8
-NGC6822
+NGC6822
+M8
 Baades
 NGC6388
 AV255</t>
@@ -2925,8 +2938,8 @@
         <is>
           <t>W28
 M20
-M8
-NGC6822
+NGC6822
+M8
 Baades
 NGC6388
 AV255</t>
@@ -2936,8 +2949,8 @@
         <is>
           <t>W28
 M20
-M8
-NGC6822
+NGC6822
+M8
 Baades
 NGC6388
 AV255</t>
@@ -3056,13 +3069,14 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="1" t="inlineStr"/>
       <c r="B2" s="1" t="inlineStr">
         <is>
           <t>NGC3199
-RCW86
-G316.75
 W28
 M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -3070,10 +3084,10 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -3081,10 +3095,10 @@
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -3092,10 +3106,10 @@
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -3103,10 +3117,10 @@
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -3114,12 +3128,12 @@
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
@@ -3128,8 +3142,8 @@
         <is>
           <t>W28
 M20
-M8
-NGC6822
+NGC6822
+M8
 Baades
 NGC6388</t>
         </is>
@@ -3138,8 +3152,8 @@
         <is>
           <t>W28
 M20
-M8
-NGC6822
+NGC6822
+M8
 Baades
 NGC6388</t>
         </is>
@@ -3178,8 +3192,8 @@
       <c r="N2" s="1" t="inlineStr">
         <is>
           <t>N44
+S308
 30Dor
-S308
 LMCclusters1
 LMCclusters2
 LMCclusters3
@@ -3279,13 +3293,14 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="1" t="inlineStr"/>
       <c r="B2" s="1" t="inlineStr">
         <is>
           <t>NGC3199
-RCW86
-G316.75
 W28
 M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -3293,10 +3308,10 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -3304,10 +3319,10 @@
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -3315,10 +3330,10 @@
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -3326,10 +3341,10 @@
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -3337,12 +3352,12 @@
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
@@ -3351,8 +3366,8 @@
         <is>
           <t>W28
 M20
-M8
-NGC6822
+NGC6822
+M8
 Baades
 NGC6388</t>
         </is>
@@ -3361,8 +3376,8 @@
         <is>
           <t>W28
 M20
-M8
-NGC6822
+NGC6822
+M8
 Baades
 NGC6388
 AV255</t>
@@ -3398,8 +3413,8 @@
       <c r="N2" s="1" t="inlineStr">
         <is>
           <t>N44
+S308
 30Dor
-S308
 LMCclusters2
 AV255</t>
         </is>
@@ -3497,13 +3512,14 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="1" t="inlineStr"/>
       <c r="B2" s="1" t="inlineStr">
         <is>
           <t>NGC3199
-RCW86
-G316.75
 W28
 M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -3511,10 +3527,10 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -3522,10 +3538,10 @@
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -3533,10 +3549,10 @@
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -3544,24 +3560,24 @@
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
@@ -3570,8 +3586,8 @@
         <is>
           <t>W28
 M20
-M8
-NGC6822
+NGC6822
+M8
 Baades
 NGC6388</t>
         </is>
@@ -3615,6 +3631,7 @@
 AV255</t>
         </is>
       </c>
+      <c r="N2" s="1" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3708,23 +3725,24 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="1" t="inlineStr"/>
       <c r="B2" s="1" t="inlineStr">
         <is>
           <t>NGC3199
-RCW86
-G316.75
 W28
 M20
+RCW86
+G316.75
 M8
 NGC6388</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -3732,10 +3750,10 @@
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -3743,32 +3761,32 @@
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 NGC6388</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 NGC6388</t>
         </is>
@@ -3819,6 +3837,7 @@
 AV255</t>
         </is>
       </c>
+      <c r="N2" s="1" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3912,64 +3931,65 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="1" t="inlineStr"/>
       <c r="B2" s="1" t="inlineStr">
         <is>
           <t>NGC3199
-RCW86
-G316.75
 W28
 M20
+RCW86
+G316.75
 M8
 NGC6388</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 NGC6388</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 NGC6388</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
+          <t>W28
+M20
 OmegaCen
+RCW86
+G316.75
+M8
 NGC6388</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 NGC6388</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 NGC6388</t>
         </is>
@@ -3990,6 +4010,7 @@
 NGC6388</t>
         </is>
       </c>
+      <c r="J2" s="1" t="inlineStr"/>
       <c r="K2" s="1" t="inlineStr">
         <is>
           <t>AV255</t>
@@ -4015,6 +4036,7 @@
 AV255</t>
         </is>
       </c>
+      <c r="N2" s="1" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4108,64 +4130,65 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="1" t="inlineStr"/>
       <c r="B2" s="1" t="inlineStr">
         <is>
           <t>NGC3199
-RCW86
-G316.75
 W28
 M20
-M8
 OmegaCen
+RCW86
+G316.75
+M8
 NGC6388</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 NGC6388</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 NGC6388</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 NGC6388</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 NGC6388</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 NGC6388</t>
         </is>
@@ -4186,6 +4209,7 @@
 NGC6388</t>
         </is>
       </c>
+      <c r="J2" s="1" t="inlineStr"/>
       <c r="K2" s="1" t="inlineStr">
         <is>
           <t>N44</t>
@@ -4207,6 +4231,7 @@
 LMCclusters2</t>
         </is>
       </c>
+      <c r="N2" s="1" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4300,37 +4325,38 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="1" t="inlineStr"/>
       <c r="B2" s="1" t="inlineStr">
         <is>
           <t>NGC3199
-RCW86
-G316.75
 W28
 M20
-M8
 OmegaCen
+RCW86
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
+          <t>W28
+M20
 OmegaCen
+RCW86
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -4338,10 +4364,10 @@
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -4349,10 +4375,10 @@
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -4360,10 +4386,10 @@
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -4416,6 +4442,7 @@
 AV255</t>
         </is>
       </c>
+      <c r="N2" s="1" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4509,12 +4536,13 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="1" t="inlineStr"/>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>RCW36
+          <t>NGC3199
+RCW36
+RCW86
 Pencil
-NGC3199
-RCW86
 G316.75
 NGC6388</t>
         </is>
@@ -4522,10 +4550,10 @@
       <c r="C2" s="1" t="inlineStr">
         <is>
           <t>NGC3199
-RCW86
-G316.75
 W28
 M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -4534,62 +4562,62 @@
       <c r="D2" s="1" t="inlineStr">
         <is>
           <t>NGC3199
-RCW86
-G316.75
 W28
 M20
-M8
 OmegaCen
+RCW86
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
+          <t>W28
+M20
 OmegaCen
+RCW86
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
 OmegaCen
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
 OmegaCen
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="H2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
@@ -4735,86 +4763,87 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="1" t="inlineStr"/>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>RCW36
+          <t>NGC3199
+OmegaCen
+RCW36
+RCW86
 Pencil
-NGC3199
-RCW86
-G316.75
+G316.75
+NGC6388</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>NGC3199
+W28
+M20
+RCW86
+G316.75
+M8
+Baades
+NGC6388</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>NGC3199
+W28
+M20
+RCW86
+G316.75
+M8
+Baades
+NGC6388</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>W28
+M20
+RCW86
+NGC6822
+G316.75
+M8
+Baades
+NGC6388</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>W28
+M20
+RCW86
+NGC6822
+G316.75
+M8
+Baades
+NGC6388</t>
+        </is>
+      </c>
+      <c r="G2" s="1" t="inlineStr">
+        <is>
+          <t>W28
+M20
 OmegaCen
-NGC6388</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>NGC3199
-RCW86
-G316.75
-W28
-M20
-M8
-Baades
-NGC6388</t>
-        </is>
-      </c>
-      <c r="D2" s="1" t="inlineStr">
-        <is>
-          <t>NGC3199
-RCW86
-G316.75
-W28
-M20
-M8
-Baades
-NGC6388</t>
-        </is>
-      </c>
-      <c r="E2" s="1" t="inlineStr">
-        <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
-Baades
-NGC6388</t>
-        </is>
-      </c>
-      <c r="F2" s="1" t="inlineStr">
-        <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
-Baades
-NGC6388</t>
-        </is>
-      </c>
-      <c r="G2" s="1" t="inlineStr">
-        <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
-OmegaCen
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="H2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
@@ -4832,8 +4861,8 @@
         <is>
           <t>W28
 M20
-M8
-NGC6822
+NGC6822
+M8
 Baades
 NGC6388</t>
         </is>
@@ -4842,8 +4871,8 @@
         <is>
           <t>W28
 M20
-M8
-NGC6822
+NGC6822
+M8
 Baades
 NGC6388
 AV255</t>
@@ -4967,38 +4996,39 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="1" t="inlineStr"/>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>RCW36
+          <t>NGC3199
+OmegaCen
+RCW36
+RCW86
 Pencil
-NGC3199
-RCW86
-G316.75
+G316.75
+Baades
+NGC6388</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>NGC3199
+W28
+M20
 OmegaCen
-Baades
-NGC6388</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="inlineStr">
+RCW86
+G316.75
+M8
+Baades
+NGC6388</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
         <is>
           <t>NGC3199
-RCW86
-G316.75
 W28
 M20
-M8
-OmegaCen
-Baades
-NGC6388</t>
-        </is>
-      </c>
-      <c r="D2" s="1" t="inlineStr">
-        <is>
-          <t>NGC3199
-RCW86
-G316.75
-W28
-M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -5006,34 +5036,34 @@
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -5041,10 +5071,10 @@
       </c>
       <c r="H2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -5054,8 +5084,8 @@
         <is>
           <t>W28
 M20
-M8
-NGC6822
+NGC6822
+M8
 Baades
 NGC6388</t>
         </is>
@@ -5064,8 +5094,8 @@
         <is>
           <t>W28
 M20
-M8
-NGC6822
+NGC6822
+M8
 Baades
 NGC6388
 AV255</t>
@@ -5075,8 +5105,8 @@
         <is>
           <t>W28
 M20
-M8
-NGC6822
+NGC6822
+M8
 Baades
 NGC6388
 AV255</t>
@@ -5196,76 +5226,77 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="1" t="inlineStr"/>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>RCW36
+          <t>NGC3199
+OmegaCen
+RCW36
+RCW86
 Pencil
-NGC3199
-RCW86
-G316.75
+G316.75
+Baades
+NGC6388</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>NGC3199
+W28
+M20
 OmegaCen
-Baades
-NGC6388</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="inlineStr">
+RCW86
+G316.75
+M8
+Baades
+NGC6388</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
         <is>
           <t>NGC3199
-RCW86
-G316.75
 W28
 M20
-M8
 OmegaCen
-Baades
-NGC6388</t>
-        </is>
-      </c>
-      <c r="D2" s="1" t="inlineStr">
-        <is>
-          <t>NGC3199
-RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+RCW86
+NGC6822
+G316.75
+M8
+Baades
+NGC6388</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>W28
+M20
 OmegaCen
-Baades
-NGC6388</t>
-        </is>
-      </c>
-      <c r="E2" s="1" t="inlineStr">
-        <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+RCW86
+NGC6822
+G316.75
+M8
+Baades
+NGC6388</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>W28
+M20
 OmegaCen
-Baades
-NGC6388</t>
-        </is>
-      </c>
-      <c r="F2" s="1" t="inlineStr">
-        <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-OmegaCen
+RCW86
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -5273,12 +5304,12 @@
       </c>
       <c r="H2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
@@ -5287,8 +5318,8 @@
         <is>
           <t>W28
 M20
-M8
-NGC6822
+NGC6822
+M8
 Baades
 NGC6388
 AV255</t>
@@ -5298,8 +5329,8 @@
         <is>
           <t>W28
 M20
-M8
-NGC6822
+NGC6822
+M8
 Baades
 NGC6388
 AV255</t>
@@ -5307,8 +5338,8 @@
       </c>
       <c r="K2" s="1" t="inlineStr">
         <is>
-          <t>M8
-NGC6822
+          <t>NGC6822
+M8
 Baades
 NGC6388
 AV255</t>
@@ -5430,27 +5461,28 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="1" t="inlineStr"/>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>RCW36
+          <t>NGC3199
+W28
+M20
+RCW36
+RCW86
 Pencil
-NGC3199
-RCW86
-G316.75
+G316.75
+M8
+Baades
+NGC6388</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>NGC3199
 W28
 M20
-M8
-Baades
-NGC6388</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>NGC3199
-RCW86
-G316.75
-W28
-M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -5458,48 +5490,48 @@
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
+          <t>W28
+M20
 OmegaCen
+RCW86
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
 OmegaCen
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
 OmegaCen
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -5507,10 +5539,10 @@
       </c>
       <c r="H2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -5520,8 +5552,8 @@
         <is>
           <t>W28
 M20
-M8
-NGC6822
+NGC6822
+M8
 Baades
 NGC6388
 AV255</t>
@@ -5531,8 +5563,8 @@
         <is>
           <t>W28
 M20
-M8
-NGC6822
+NGC6822
+M8
 Baades
 NGC6388
 AV255</t>
@@ -5659,28 +5691,29 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="1" t="inlineStr"/>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>RCW36
+          <t>NGC3199
+W28
+M20
+OmegaCen
+RCW36
+RCW86
 Pencil
-NGC3199
-RCW86
-G316.75
+G316.75
+M8
+Baades
+NGC6388</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>NGC3199
 W28
 M20
-M8
-OmegaCen
-Baades
-NGC6388</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>NGC3199
-RCW86
-G316.75
-W28
-M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -5688,10 +5721,10 @@
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -5699,34 +5732,34 @@
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -5734,10 +5767,10 @@
       </c>
       <c r="H2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
+          <t>W28
+M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -5756,8 +5789,8 @@
         <is>
           <t>W28
 M20
-M8
-NGC6822
+NGC6822
+M8
 Baades
 NGC6388
 AV255</t>
@@ -5887,27 +5920,28 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" s="1" t="inlineStr"/>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>RCW36
+          <t>NGC3199
+W28
+M20
+RCW36
+RCW86
 Pencil
-NGC3199
-RCW86
-G316.75
+G316.75
+M8
+Baades
+NGC6388</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>NGC3199
 W28
 M20
-M8
-Baades
-NGC6388</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>NGC3199
-RCW86
-G316.75
-W28
-M20
+RCW86
+G316.75
 M8
 Baades
 NGC6388</t>
@@ -5915,61 +5949,61 @@
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
+          <t>W28
+M20
 OmegaCen
+RCW86
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
+          <t>W28
+M20
 OmegaCen
+RCW86
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
 OmegaCen
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>
       </c>
       <c r="H2" s="1" t="inlineStr">
         <is>
-          <t>RCW86
-G316.75
-W28
-M20
-M8
-NGC6822
+          <t>W28
+M20
+RCW86
+NGC6822
+G316.75
+M8
 Baades
 NGC6388</t>
         </is>

</xml_diff>